<commit_message>
Add graphics group talk and new MS students
</commit_message>
<xml_diff>
--- a/CV.xlsx
+++ b/CV.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Education" sheetId="1" state="visible" r:id="rId2"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="609">
   <si>
     <t xml:space="preserve">degree</t>
   </si>
@@ -1273,6 +1273,18 @@
     <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/02-graphics-cv/xlsx-tex-bib-pdf.svg</t>
   </si>
   <si>
+    <t xml:space="preserve">Building a CV/Blog Automatically</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This week will be the second of a 2-part workshop.    On Feb 15, we talked about how to make a CV with R and a google spreadsheet (and why you might want to do so).    This week, we'll talk about how to use this same setup to build a blog-type website with posts for each paper and presentation, using quarto.    Setup steps:        1. Clone or fork the github repository I've made: https://github.com/srvanderplas/cv-site-template.     2. Modify the data/CV.bib file in the repository to contain your publications, if you want to include them on the CV.      3. Modify the data/CV.xlsx file in the repository to contain your talks    During the presentation, I'll walk you through the workflow I use and show you how to use the code I've written to create your own CV-style blog from a spreadsheet and a bib file.   We'll also talk about how to use this workflow, git submodules, and github actions to automatically keep things updated. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/03-graphics-blog/#/title-slide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/03-graphics-blog/talk-post-layout.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">year</t>
   </si>
   <si>
@@ -1562,6 +1574,18 @@
   </si>
   <si>
     <t xml:space="preserve">A Statistical Approach to Learning Computer Vision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University of Nebraska – Lincoln</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maksuda Atka Toma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An Historical Analysis of Pie and Bar Chart Experiments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dinuwanthi Lianage</t>
   </si>
   <si>
     <t xml:space="preserve">Student Name</t>
@@ -1969,7 +1993,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1991,11 +2015,19 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -2028,6 +2060,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -2311,7 +2347,7 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>164</v>
@@ -2320,103 +2356,103 @@
         <v>166</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="H1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="n">
+      <c r="A2" s="10" t="n">
         <v>20140901</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="n">
+        <v>20140501</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="n">
-        <v>20140501</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>445</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="n">
+        <v>20130801</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="n">
-        <v>20130801</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>445</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10" t="n">
+        <v>20130501</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="n">
-        <v>20130501</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>445</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -2425,22 +2461,22 @@
         <v>20220117</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>251</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2448,22 +2484,22 @@
         <v>20220516</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>251</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2471,22 +2507,22 @@
         <v>20230116</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>251</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2494,22 +2530,22 @@
         <v>20240117</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>251</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -2538,13 +2574,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>34</v>
@@ -2559,7 +2595,7 @@
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="I1" s="1"/>
     </row>
@@ -2579,17 +2615,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="20.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="20.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2597,25 +2633,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>127</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2635,18 +2671,18 @@
         <v>2019</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -2658,15 +2694,15 @@
         <v>2019</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
@@ -2681,13 +2717,13 @@
         <v>2018</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2707,13 +2743,13 @@
         <v>2020</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2733,21 +2769,21 @@
         <v>2020</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>12</v>
@@ -2759,15 +2795,15 @@
         <v>2019</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
@@ -2782,18 +2818,18 @@
         <v>2019</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>12</v>
@@ -2805,10 +2841,10 @@
         <v>2019</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2831,10 +2867,10 @@
         <v>113</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2854,10 +2890,10 @@
         <v>2020</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2877,13 +2913,13 @@
         <v>2023</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2903,13 +2939,13 @@
         <v>2023</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2929,18 +2965,18 @@
         <v>2022</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>250</v>
@@ -2952,13 +2988,13 @@
         <v>2021</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2978,10 +3014,10 @@
         <v>2024</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3001,10 +3037,10 @@
         <v>2023</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3024,10 +3060,10 @@
         <v>2023</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3047,13 +3083,13 @@
         <v>0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3073,10 +3109,10 @@
         <v>0</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3096,10 +3132,10 @@
         <v>0</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3119,10 +3155,10 @@
         <v>0</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3139,13 +3175,56 @@
         <v>2023</v>
       </c>
       <c r="E23" s="1" t="n">
-        <v>2025</v>
+        <v>0</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>505</v>
+        <v>509</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>513</v>
       </c>
     </row>
   </sheetData>
@@ -3174,16 +3253,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>506</v>
+        <v>514</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>289</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>507</v>
+        <v>515</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>508</v>
+        <v>516</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>14</v>
@@ -3191,10 +3270,10 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>509</v>
+        <v>517</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>510</v>
+        <v>518</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>45007</v>
@@ -3205,15 +3284,15 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>511</v>
+        <v>519</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="15" t="n">
+      <c r="C3" s="18" t="n">
         <v>44774</v>
       </c>
-      <c r="D3" s="15" t="n">
+      <c r="D3" s="18" t="n">
         <v>45047</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -3222,15 +3301,15 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>512</v>
+        <v>520</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="15" t="n">
+      <c r="C4" s="18" t="n">
         <v>44774</v>
       </c>
-      <c r="D4" s="15" t="n">
+      <c r="D4" s="18" t="n">
         <v>45047</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -3239,15 +3318,15 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>513</v>
+        <v>521</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="16" t="n">
+      <c r="C5" s="19" t="n">
         <v>44835</v>
       </c>
-      <c r="D5" s="15" t="n">
+      <c r="D5" s="18" t="n">
         <v>45047</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -3256,12 +3335,12 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>514</v>
+        <v>522</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="15" t="n">
+      <c r="C6" s="18" t="n">
         <v>44409</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -3302,19 +3381,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>515</v>
+        <v>523</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>516</v>
+        <v>524</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>127</v>
@@ -3322,9 +3401,9 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="B2" s="1" t="b">
+        <v>525</v>
+      </c>
+      <c r="B2" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3335,20 +3414,20 @@
         <v>2019</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>518</v>
+        <v>526</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>175</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>519</v>
+        <v>527</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="B3" s="1" t="b">
+        <v>525</v>
+      </c>
+      <c r="B3" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3359,20 +3438,20 @@
         <v>2021</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>520</v>
+        <v>528</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>521</v>
+        <v>529</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>519</v>
+        <v>527</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="B4" s="1" t="b">
+        <v>525</v>
+      </c>
+      <c r="B4" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3383,23 +3462,23 @@
         <v>2019</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>522</v>
+        <v>530</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>523</v>
+        <v>531</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>524</v>
+        <v>532</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>525</v>
+        <v>533</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B5" s="1" t="b">
+      <c r="B5" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3410,23 +3489,23 @@
         <v>2020</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>520</v>
+        <v>528</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>526</v>
+        <v>534</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>527</v>
+        <v>535</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>528</v>
+        <v>536</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="B6" s="1" t="b">
+        <v>525</v>
+      </c>
+      <c r="B6" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3437,17 +3516,17 @@
         <v>2026</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>529</v>
+        <v>537</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>530</v>
+        <v>538</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="B7" s="1" t="b">
+        <v>525</v>
+      </c>
+      <c r="B7" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3458,20 +3537,20 @@
         <v>2022</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>531</v>
+        <v>539</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>175</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>519</v>
+        <v>527</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="B8" s="1" t="b">
+        <v>525</v>
+      </c>
+      <c r="B8" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3482,17 +3561,17 @@
         <v>2020</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>532</v>
+        <v>540</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>533</v>
+        <v>541</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B9" s="1" t="b">
+      <c r="B9" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3503,20 +3582,20 @@
         <v>2021</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>534</v>
+        <v>542</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>527</v>
+        <v>535</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="B10" s="1" t="b">
+        <v>543</v>
+      </c>
+      <c r="B10" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3527,20 +3606,20 @@
         <v>2020</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>536</v>
+        <v>544</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>537</v>
+        <v>545</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>538</v>
+        <v>546</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="B11" s="1" t="b">
+        <v>525</v>
+      </c>
+      <c r="B11" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3551,17 +3630,17 @@
         <v>2024</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>529</v>
+        <v>537</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>539</v>
+        <v>547</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B12" s="1" t="b">
+      <c r="B12" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3572,23 +3651,23 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>540</v>
+        <v>548</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>541</v>
+        <v>549</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>542</v>
+        <v>550</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>543</v>
+        <v>551</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="B13" s="1" t="b">
+        <v>543</v>
+      </c>
+      <c r="B13" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3599,20 +3678,20 @@
         <v>2022</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>544</v>
+        <v>552</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>545</v>
+        <v>553</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>546</v>
+        <v>554</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B14" s="1" t="b">
+      <c r="B14" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3623,17 +3702,17 @@
         <v>2022</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>520</v>
+        <v>528</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>547</v>
+        <v>555</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="B15" s="1" t="b">
+        <v>543</v>
+      </c>
+      <c r="B15" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3644,17 +3723,17 @@
         <v>2021</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>520</v>
+        <v>528</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>548</v>
+        <v>556</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="B16" s="1" t="b">
+        <v>543</v>
+      </c>
+      <c r="B16" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3665,20 +3744,20 @@
         <v>2021</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>520</v>
+        <v>528</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>549</v>
+        <v>557</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>550</v>
+        <v>558</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="B17" s="1" t="b">
+        <v>525</v>
+      </c>
+      <c r="B17" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3689,20 +3768,20 @@
         <v>2023</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>551</v>
+        <v>559</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>175</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>519</v>
+        <v>527</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="B18" s="1" t="b">
+        <v>543</v>
+      </c>
+      <c r="B18" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3713,20 +3792,20 @@
         <v>0</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>552</v>
+        <v>560</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>527</v>
+        <v>535</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>553</v>
+        <v>561</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="B19" s="1" t="b">
+        <v>525</v>
+      </c>
+      <c r="B19" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3737,20 +3816,20 @@
         <v>2025</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>520</v>
+        <v>528</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>554</v>
+        <v>562</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>519</v>
+        <v>527</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="B20" s="1" t="b">
+        <v>525</v>
+      </c>
+      <c r="B20" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3761,20 +3840,20 @@
         <v>2024</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>555</v>
+        <v>563</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>175</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>519</v>
+        <v>527</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="B21" s="1" t="b">
+        <v>543</v>
+      </c>
+      <c r="B21" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3785,13 +3864,13 @@
         <v>0</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>520</v>
+        <v>528</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>553</v>
+        <v>561</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3828,10 +3907,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>557</v>
+        <v>565</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3839,7 +3918,7 @@
         <v>2022</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>539</v>
+        <v>547</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3847,7 +3926,7 @@
         <v>2019</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>530</v>
+        <v>538</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3855,7 +3934,7 @@
         <v>2020</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>558</v>
+        <v>566</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3863,7 +3942,7 @@
         <v>2020</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>559</v>
+        <v>567</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3871,7 +3950,7 @@
         <v>2020</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>560</v>
+        <v>568</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3879,7 +3958,7 @@
         <v>2021</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>561</v>
+        <v>569</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3887,7 +3966,7 @@
         <v>2021</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>562</v>
+        <v>570</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3895,7 +3974,7 @@
         <v>2021</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>563</v>
+        <v>571</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3903,7 +3982,7 @@
         <v>2022</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>564</v>
+        <v>572</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3911,7 +3990,7 @@
         <v>2020</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>565</v>
+        <v>573</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3919,7 +3998,7 @@
         <v>2021</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>565</v>
+        <v>573</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3927,7 +4006,7 @@
         <v>2022</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>565</v>
+        <v>573</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3935,7 +4014,7 @@
         <v>2023</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>565</v>
+        <v>573</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3943,7 +4022,7 @@
         <v>2022</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>561</v>
+        <v>569</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3951,7 +4030,7 @@
         <v>2023</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>539</v>
+        <v>547</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3959,7 +4038,7 @@
         <v>2023</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>566</v>
+        <v>574</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3967,7 +4046,7 @@
         <v>2023</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>530</v>
+        <v>538</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3975,7 +4054,7 @@
         <v>2023</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>539</v>
+        <v>547</v>
       </c>
     </row>
   </sheetData>
@@ -4007,26 +4086,26 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>567</v>
+        <v>575</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>568</v>
+        <v>576</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>127</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>569</v>
+        <v>577</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>570</v>
+        <v>578</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>571</v>
+        <v>579</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="b">
+      <c r="A2" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4037,14 +4116,14 @@
         <v>2023</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>572</v>
+        <v>580</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>573</v>
+        <v>581</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="b">
+      <c r="A3" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4055,14 +4134,14 @@
         <v>2023</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>574</v>
+        <v>582</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>575</v>
+        <v>583</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="b">
+      <c r="A4" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4073,14 +4152,14 @@
         <v>2022</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>576</v>
+        <v>584</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>577</v>
+        <v>585</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="b">
+      <c r="A5" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4091,11 +4170,11 @@
         <v>2020</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>578</v>
+        <v>586</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="b">
+      <c r="A6" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4106,10 +4185,10 @@
         <v>2020</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>579</v>
+        <v>587</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>580</v>
+        <v>588</v>
       </c>
     </row>
   </sheetData>
@@ -4144,10 +4223,10 @@
         <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>567</v>
+        <v>575</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>568</v>
+        <v>576</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>127</v>
@@ -4156,40 +4235,40 @@
         <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>569</v>
+        <v>577</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>570</v>
+        <v>578</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>571</v>
+        <v>579</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="b">
+      <c r="A2" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="C2" s="8" t="n">
+        <v>589</v>
+      </c>
+      <c r="C2" s="10" t="n">
         <v>2023</v>
       </c>
-      <c r="D2" s="8" t="n">
+      <c r="D2" s="10" t="n">
         <v>2023</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>582</v>
+        <v>590</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>583</v>
+        <v>591</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -4197,27 +4276,27 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="b">
+      <c r="A3" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="C3" s="8" t="n">
+        <v>589</v>
+      </c>
+      <c r="C3" s="10" t="n">
         <v>2022</v>
       </c>
-      <c r="D3" s="8" t="n">
+      <c r="D3" s="10" t="n">
         <v>2022</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>586</v>
+        <v>594</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>587</v>
+        <v>595</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -4225,27 +4304,27 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="b">
+      <c r="A4" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="C4" s="8" t="n">
+        <v>589</v>
+      </c>
+      <c r="C4" s="10" t="n">
         <v>2022</v>
       </c>
-      <c r="D4" s="8" t="n">
+      <c r="D4" s="10" t="n">
         <v>2022</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>588</v>
+        <v>596</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>589</v>
+        <v>597</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -4253,27 +4332,27 @@
       <c r="L4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="b">
+      <c r="A5" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="C5" s="8" t="n">
+        <v>589</v>
+      </c>
+      <c r="C5" s="10" t="n">
         <v>2022</v>
       </c>
-      <c r="D5" s="8" t="n">
+      <c r="D5" s="10" t="n">
         <v>2022</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>582</v>
+        <v>590</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>590</v>
+        <v>598</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>591</v>
+        <v>599</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -4281,27 +4360,27 @@
       <c r="L5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="b">
+      <c r="A6" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="C6" s="8" t="n">
+        <v>589</v>
+      </c>
+      <c r="C6" s="10" t="n">
         <v>2021</v>
       </c>
-      <c r="D6" s="8" t="n">
+      <c r="D6" s="10" t="n">
         <v>2021</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>582</v>
+        <v>590</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>590</v>
+        <v>598</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>592</v>
+        <v>600</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -4310,27 +4389,27 @@
       <c r="L6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="b">
+      <c r="A7" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>593</v>
-      </c>
-      <c r="C7" s="8" t="n">
+        <v>601</v>
+      </c>
+      <c r="C7" s="10" t="n">
         <v>2021</v>
       </c>
-      <c r="D7" s="8" t="n">
+      <c r="D7" s="10" t="n">
         <v>2021</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>594</v>
+        <v>602</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>596</v>
+        <v>604</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -4339,27 +4418,27 @@
       <c r="L7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="b">
+      <c r="A8" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>593</v>
-      </c>
-      <c r="C8" s="8" t="n">
+        <v>601</v>
+      </c>
+      <c r="C8" s="10" t="n">
         <v>2021</v>
       </c>
-      <c r="D8" s="8" t="n">
+      <c r="D8" s="10" t="n">
         <v>2021</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>319</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>597</v>
+        <v>605</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -4368,30 +4447,30 @@
       <c r="L8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="b">
+      <c r="A9" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>593</v>
-      </c>
-      <c r="C9" s="8" t="n">
+        <v>601</v>
+      </c>
+      <c r="C9" s="10" t="n">
         <v>2020</v>
       </c>
-      <c r="D9" s="8" t="n">
+      <c r="D9" s="10" t="n">
         <v>2020</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>600</v>
+        <v>608</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -4674,14 +4753,14 @@
       <c r="AD1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="b">
+      <c r="A2" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="5" t="b">
+      <c r="C2" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4726,14 +4805,14 @@
       <c r="AD2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="b">
+      <c r="A3" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="5" t="b">
+      <c r="C3" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4774,14 +4853,14 @@
       <c r="AD3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="b">
+      <c r="A4" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="5" t="b">
+      <c r="C4" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4826,14 +4905,14 @@
       <c r="AD4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="b">
+      <c r="A5" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="5" t="b">
+      <c r="C5" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4878,14 +4957,14 @@
       <c r="AD5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="b">
+      <c r="A6" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="5" t="b">
+      <c r="C6" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4930,14 +5009,14 @@
       <c r="AD6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="b">
+      <c r="A7" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="5" t="b">
+      <c r="C7" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4982,14 +5061,14 @@
       <c r="AD7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="b">
+      <c r="A8" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="1" t="b">
+      <c r="C8" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5030,14 +5109,14 @@
       <c r="AD8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="b">
+      <c r="A9" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="1" t="b">
+      <c r="C9" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5058,14 +5137,14 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="b">
+      <c r="A10" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="1" t="b">
+      <c r="C10" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5086,14 +5165,14 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="b">
+      <c r="A11" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="1" t="b">
+      <c r="C11" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5134,7 +5213,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="31.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="7" width="31.38"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5182,7 +5261,7 @@
       <c r="A2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="1" t="b">
+      <c r="B2" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5204,7 +5283,7 @@
       <c r="H2" s="1" t="n">
         <v>299859</v>
       </c>
-      <c r="I2" s="1" t="b">
+      <c r="I2" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5223,7 +5302,7 @@
       <c r="A3" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="1" t="b">
+      <c r="B3" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5245,7 +5324,7 @@
       <c r="H3" s="1" t="n">
         <v>380650</v>
       </c>
-      <c r="I3" s="1" t="b">
+      <c r="I3" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5261,7 +5340,7 @@
       <c r="A4" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="1" t="b">
+      <c r="B4" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5283,7 +5362,7 @@
       <c r="H4" s="1" t="n">
         <v>20000000</v>
       </c>
-      <c r="I4" s="1" t="b">
+      <c r="I4" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5302,7 +5381,7 @@
       <c r="A5" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="1" t="b">
+      <c r="B5" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5324,7 +5403,7 @@
       <c r="H5" s="1" t="n">
         <v>4000000</v>
       </c>
-      <c r="I5" s="1" t="b">
+      <c r="I5" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5345,7 +5424,7 @@
       <c r="A6" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="1" t="b">
+      <c r="B6" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5367,7 +5446,7 @@
       <c r="H6" s="1" t="n">
         <v>300000</v>
       </c>
-      <c r="I6" s="1" t="b">
+      <c r="I6" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5382,7 +5461,7 @@
       <c r="A7" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B7" s="1" t="b">
+      <c r="B7" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5404,7 +5483,7 @@
       <c r="H7" s="1" t="n">
         <v>1500000</v>
       </c>
-      <c r="I7" s="1" t="b">
+      <c r="I7" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5422,7 +5501,7 @@
       <c r="A8" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="1" t="b">
+      <c r="B8" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5444,7 +5523,7 @@
       <c r="H8" s="1" t="n">
         <v>197699</v>
       </c>
-      <c r="I8" s="1" t="b">
+      <c r="I8" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5462,7 +5541,7 @@
       <c r="A9" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="1" t="b">
+      <c r="B9" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5484,7 +5563,7 @@
       <c r="H9" s="1" t="n">
         <v>300000</v>
       </c>
-      <c r="I9" s="1" t="b">
+      <c r="I9" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5493,7 +5572,7 @@
       <c r="A10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="1" t="b">
+      <c r="B10" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5515,7 +5594,7 @@
       <c r="H10" s="1" t="n">
         <v>20000000</v>
       </c>
-      <c r="I10" s="1" t="b">
+      <c r="I10" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5527,7 +5606,7 @@
       <c r="A11" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="1" t="b">
+      <c r="B11" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5549,7 +5628,7 @@
       <c r="H11" s="1" t="n">
         <v>3000000</v>
       </c>
-      <c r="I11" s="1" t="b">
+      <c r="I11" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5558,7 +5637,7 @@
       <c r="A12" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="1" t="b">
+      <c r="B12" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5580,7 +5659,7 @@
       <c r="H12" s="1" t="n">
         <v>281755</v>
       </c>
-      <c r="I12" s="1" t="b">
+      <c r="I12" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5589,7 +5668,7 @@
       <c r="A13" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="1" t="b">
+      <c r="B13" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5602,7 +5681,7 @@
       <c r="E13" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="8" t="s">
         <v>100</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -5611,13 +5690,13 @@
       <c r="H13" s="1" t="n">
         <v>666485</v>
       </c>
-      <c r="I13" s="1" t="b">
+      <c r="I13" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F14" s="7"/>
+      <c r="F14" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5740,21 +5819,21 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="b">
+      <c r="A2" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="5" t="b">
+      <c r="C2" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D2" s="8" t="n">
+      <c r="D2" s="10" t="n">
         <v>2021</v>
       </c>
-      <c r="E2" s="8" t="n">
+      <c r="E2" s="10" t="n">
         <v>2021</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -5763,26 +5842,26 @@
       <c r="G2" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="b">
+      <c r="A3" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="5" t="b">
+      <c r="C3" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D3" s="8" t="n">
+      <c r="D3" s="10" t="n">
         <v>2012</v>
       </c>
-      <c r="E3" s="8" t="n">
+      <c r="E3" s="10" t="n">
         <v>2012</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -5793,21 +5872,21 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="b">
+      <c r="A4" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C4" s="5" t="b">
+      <c r="C4" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D4" s="8" t="n">
+      <c r="D4" s="10" t="n">
         <v>2009</v>
       </c>
-      <c r="E4" s="8" t="n">
+      <c r="E4" s="10" t="n">
         <v>2011</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -5819,21 +5898,21 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="b">
+      <c r="A5" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C5" s="5" t="b">
+      <c r="C5" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D5" s="8" t="n">
+      <c r="D5" s="10" t="n">
         <v>2005</v>
       </c>
-      <c r="E5" s="8" t="n">
+      <c r="E5" s="10" t="n">
         <v>2009</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -5845,21 +5924,21 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="b">
+      <c r="A6" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C6" s="5" t="b">
+      <c r="C6" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D6" s="8" t="n">
+      <c r="D6" s="10" t="n">
         <v>2009</v>
       </c>
-      <c r="E6" s="8" t="n">
+      <c r="E6" s="10" t="n">
         <v>2009</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -5871,21 +5950,21 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="b">
+      <c r="A7" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C7" s="5" t="b">
+      <c r="C7" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D7" s="8" t="n">
+      <c r="D7" s="10" t="n">
         <v>2009</v>
       </c>
-      <c r="E7" s="8" t="n">
+      <c r="E7" s="10" t="n">
         <v>2009</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -5897,21 +5976,21 @@
       <c r="H7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="b">
+      <c r="A8" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C8" s="5" t="b">
+      <c r="C8" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D8" s="8" t="n">
+      <c r="D8" s="10" t="n">
         <v>2006</v>
       </c>
-      <c r="E8" s="8" t="n">
+      <c r="E8" s="10" t="n">
         <v>2009</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -5923,21 +6002,21 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="b">
+      <c r="A9" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C9" s="5" t="b">
+      <c r="C9" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D9" s="8" t="n">
+      <c r="D9" s="10" t="n">
         <v>2005</v>
       </c>
-      <c r="E9" s="8" t="n">
+      <c r="E9" s="10" t="n">
         <v>2009</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -5949,21 +6028,21 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="b">
+      <c r="A10" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C10" s="5" t="b">
+      <c r="C10" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D10" s="8" t="n">
+      <c r="D10" s="10" t="n">
         <v>2005</v>
       </c>
-      <c r="E10" s="8" t="n">
+      <c r="E10" s="10" t="n">
         <v>2005</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -5975,21 +6054,21 @@
       <c r="H10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="b">
+      <c r="A11" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C11" s="5" t="b">
+      <c r="C11" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D11" s="8" t="n">
+      <c r="D11" s="10" t="n">
         <v>2005</v>
       </c>
-      <c r="E11" s="8" t="n">
+      <c r="E11" s="10" t="n">
         <v>2005</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -6025,7 +6104,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="9"/>
+      <c r="G14" s="11"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6064,7 +6143,7 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="9"/>
+      <c r="F18" s="11"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
@@ -6074,7 +6153,7 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="9"/>
+      <c r="F19" s="11"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
@@ -6129,7 +6208,7 @@
       <c r="C2" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="12" t="s">
         <v>133</v>
       </c>
     </row>
@@ -6143,7 +6222,7 @@
       <c r="C3" s="1" t="n">
         <v>2020</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="12" t="s">
         <v>136</v>
       </c>
     </row>
@@ -6160,7 +6239,7 @@
       <c r="D4" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="12" t="s">
         <v>139</v>
       </c>
     </row>
@@ -6174,7 +6253,7 @@
       <c r="C5" s="1" t="n">
         <v>2019</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="12" t="s">
         <v>142</v>
       </c>
     </row>
@@ -6188,7 +6267,7 @@
       <c r="C6" s="1" t="n">
         <v>2018</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="12" t="s">
         <v>145</v>
       </c>
     </row>
@@ -6202,7 +6281,7 @@
       <c r="C7" s="1" t="n">
         <v>2018</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="12" t="s">
         <v>148</v>
       </c>
     </row>
@@ -6216,7 +6295,7 @@
       <c r="C8" s="1" t="n">
         <v>2018</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="12" t="s">
         <v>151</v>
       </c>
     </row>
@@ -6233,7 +6312,7 @@
       <c r="D9" s="1" t="n">
         <v>2020</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="12" t="s">
         <v>154</v>
       </c>
     </row>
@@ -6250,7 +6329,7 @@
       <c r="D10" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="12" t="s">
         <v>157</v>
       </c>
     </row>
@@ -6267,7 +6346,7 @@
       <c r="D11" s="1" t="n">
         <v>2015</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="12" t="s">
         <v>160</v>
       </c>
     </row>
@@ -6299,19 +6378,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K38" activeCellId="0" sqref="K38"/>
+      <selection pane="bottomLeft" activeCell="M44" activeCellId="0" sqref="M44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="15.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="14.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="15.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="15.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="14.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="7" width="15.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6403,13 +6482,13 @@
       <c r="H3" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="12" t="s">
         <v>182</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="12" t="s">
         <v>184</v>
       </c>
     </row>
@@ -6438,13 +6517,13 @@
       <c r="H4" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="12" t="s">
         <v>188</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="12" t="s">
         <v>190</v>
       </c>
     </row>
@@ -6473,16 +6552,16 @@
       <c r="H5" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="12" t="s">
         <v>194</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="12" t="s">
         <v>196</v>
       </c>
     </row>
@@ -6514,13 +6593,13 @@
       <c r="I6" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="12" t="s">
         <v>201</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="12" t="s">
         <v>202</v>
       </c>
     </row>
@@ -6578,16 +6657,16 @@
       <c r="H8" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="12" t="s">
         <v>210</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="L8" s="12" t="s">
         <v>212</v>
       </c>
     </row>
@@ -6645,16 +6724,16 @@
       <c r="H10" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="12" t="s">
         <v>219</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="L10" s="10" t="s">
+      <c r="L10" s="12" t="s">
         <v>220</v>
       </c>
     </row>
@@ -6686,13 +6765,13 @@
       <c r="I11" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="J11" s="12" t="s">
         <v>224</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="L11" s="10" t="s">
+      <c r="L11" s="12" t="s">
         <v>226</v>
       </c>
     </row>
@@ -6724,13 +6803,13 @@
       <c r="I12" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="J12" s="12" t="s">
         <v>230</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="L12" s="10" t="s">
+      <c r="L12" s="12" t="s">
         <v>232</v>
       </c>
     </row>
@@ -6759,13 +6838,13 @@
       <c r="I13" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="12" t="s">
         <v>237</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="L13" s="10" t="s">
+      <c r="L13" s="12" t="s">
         <v>239</v>
       </c>
     </row>
@@ -6794,13 +6873,13 @@
       <c r="H14" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="J14" s="12" t="s">
         <v>244</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="L14" s="10" t="s">
+      <c r="L14" s="12" t="s">
         <v>246</v>
       </c>
     </row>
@@ -6829,13 +6908,13 @@
       <c r="H15" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="J15" s="10" t="s">
+      <c r="J15" s="12" t="s">
         <v>252</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="L15" s="10" t="s">
+      <c r="L15" s="12" t="s">
         <v>254</v>
       </c>
     </row>
@@ -6867,13 +6946,13 @@
       <c r="I16" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="J16" s="12" t="s">
         <v>260</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="L16" s="10" t="s">
+      <c r="L16" s="12" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6902,13 +6981,13 @@
       <c r="H17" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="J17" s="13" t="s">
+      <c r="J17" s="15" t="s">
         <v>266</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="L17" s="10" t="s">
+      <c r="L17" s="12" t="s">
         <v>268</v>
       </c>
     </row>
@@ -6934,13 +7013,13 @@
       <c r="H18" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="J18" s="13" t="s">
+      <c r="J18" s="15" t="s">
         <v>272</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="L18" s="10" t="s">
+      <c r="L18" s="12" t="s">
         <v>274</v>
       </c>
     </row>
@@ -6969,13 +7048,13 @@
       <c r="H19" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="J19" s="13" t="s">
+      <c r="J19" s="15" t="s">
         <v>277</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="L19" s="10" t="s">
+      <c r="L19" s="12" t="s">
         <v>279</v>
       </c>
     </row>
@@ -7007,13 +7086,13 @@
       <c r="I20" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="J20" s="13" t="s">
+      <c r="J20" s="15" t="s">
         <v>284</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="L20" s="10" t="s">
+      <c r="L20" s="12" t="s">
         <v>286</v>
       </c>
     </row>
@@ -7045,13 +7124,13 @@
       <c r="I21" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="J21" s="13" t="s">
+      <c r="J21" s="15" t="s">
         <v>292</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="L21" s="10" t="s">
+      <c r="L21" s="12" t="s">
         <v>294</v>
       </c>
     </row>
@@ -7083,13 +7162,13 @@
       <c r="I22" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="J22" s="13" t="s">
+      <c r="J22" s="15" t="s">
         <v>301</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="L22" s="10" t="s">
+      <c r="L22" s="12" t="s">
         <v>303</v>
       </c>
     </row>
@@ -7115,13 +7194,13 @@
       <c r="H23" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="J23" s="13" t="s">
+      <c r="J23" s="15" t="s">
         <v>306</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="L23" s="10" t="s">
+      <c r="L23" s="12" t="s">
         <v>307</v>
       </c>
     </row>
@@ -7153,13 +7232,13 @@
       <c r="I24" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="J24" s="13" t="s">
+      <c r="J24" s="15" t="s">
         <v>311</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="L24" s="10" t="s">
+      <c r="L24" s="12" t="s">
         <v>313</v>
       </c>
     </row>
@@ -7191,13 +7270,13 @@
       <c r="I25" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="J25" s="10" t="s">
+      <c r="J25" s="12" t="s">
         <v>315</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="L25" s="10" t="s">
+      <c r="L25" s="12" t="s">
         <v>316</v>
       </c>
     </row>
@@ -7225,13 +7304,13 @@
         <v>258</v>
       </c>
       <c r="I26" s="1"/>
-      <c r="J26" s="10" t="s">
+      <c r="J26" s="12" t="s">
         <v>321</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="L26" s="10" t="s">
+      <c r="L26" s="12" t="s">
         <v>323</v>
       </c>
     </row>
@@ -7263,13 +7342,13 @@
       <c r="I27" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="J27" s="10" t="s">
+      <c r="J27" s="12" t="s">
         <v>328</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="L27" s="10" t="s">
+      <c r="L27" s="12" t="s">
         <v>329</v>
       </c>
     </row>
@@ -7327,13 +7406,13 @@
       <c r="I29" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="J29" s="10" t="s">
+      <c r="J29" s="12" t="s">
         <v>337</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="L29" s="10" t="s">
+      <c r="L29" s="12" t="s">
         <v>338</v>
       </c>
     </row>
@@ -7365,13 +7444,13 @@
       <c r="I30" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="J30" s="10" t="s">
+      <c r="J30" s="12" t="s">
         <v>342</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="L30" s="10" t="s">
+      <c r="L30" s="12" t="s">
         <v>344</v>
       </c>
     </row>
@@ -7403,13 +7482,13 @@
       <c r="I31" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="J31" s="10" t="s">
+      <c r="J31" s="12" t="s">
         <v>347</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="L31" s="10" t="s">
+      <c r="L31" s="12" t="s">
         <v>349</v>
       </c>
     </row>
@@ -7441,13 +7520,13 @@
       <c r="I32" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="J32" s="10" t="s">
+      <c r="J32" s="12" t="s">
         <v>353</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="L32" s="10" t="s">
+      <c r="L32" s="12" t="s">
         <v>354</v>
       </c>
     </row>
@@ -7476,13 +7555,13 @@
       <c r="H33" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="J33" s="10" t="s">
+      <c r="J33" s="12" t="s">
         <v>357</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="L33" s="10" t="s">
+      <c r="L33" s="12" t="s">
         <v>359</v>
       </c>
     </row>
@@ -7511,13 +7590,13 @@
       <c r="H34" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="J34" s="10" t="s">
+      <c r="J34" s="12" t="s">
         <v>362</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="L34" s="10" t="s">
+      <c r="L34" s="12" t="s">
         <v>363</v>
       </c>
     </row>
@@ -7549,13 +7628,13 @@
       <c r="I35" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="J35" s="10" t="s">
+      <c r="J35" s="12" t="s">
         <v>368</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="L35" s="10" t="s">
+      <c r="L35" s="12" t="s">
         <v>370</v>
       </c>
     </row>
@@ -7584,13 +7663,13 @@
       <c r="I36" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="J36" s="10" t="s">
+      <c r="J36" s="12" t="s">
         <v>376</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="L36" s="10" t="s">
+      <c r="L36" s="12" t="s">
         <v>378</v>
       </c>
     </row>
@@ -7622,13 +7701,13 @@
       <c r="I37" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="J37" s="10" t="s">
+      <c r="J37" s="12" t="s">
         <v>385</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="L37" s="10" t="s">
+      <c r="L37" s="12" t="s">
         <v>387</v>
       </c>
     </row>
@@ -7654,13 +7733,13 @@
       <c r="H38" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="J38" s="10" t="s">
+      <c r="J38" s="12" t="s">
         <v>390</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="L38" s="10" t="s">
+      <c r="L38" s="12" t="s">
         <v>392</v>
       </c>
     </row>
@@ -7689,7 +7768,7 @@
       <c r="I39" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="J39" s="10" t="s">
+      <c r="J39" s="12" t="s">
         <v>397</v>
       </c>
       <c r="K39" s="1" t="s">
@@ -7724,13 +7803,13 @@
       <c r="I40" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="J40" s="10" t="s">
+      <c r="J40" s="12" t="s">
         <v>401</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="L40" s="10" t="s">
+      <c r="L40" s="12" t="s">
         <v>403</v>
       </c>
     </row>
@@ -7759,17 +7838,55 @@
       <c r="H41" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="I41" s="14" t="s">
+      <c r="I41" s="16" t="s">
         <v>405</v>
       </c>
-      <c r="J41" s="10" t="s">
+      <c r="J41" s="12" t="s">
         <v>406</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="L41" s="10" t="s">
+      <c r="L41" s="12" t="s">
         <v>408</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="17" t="n">
+        <v>45358</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="I42" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="J42" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="L42" s="0" t="s">
+        <v>412</v>
       </c>
     </row>
   </sheetData>
@@ -7871,41 +7988,41 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="6" width="25.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="48.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="7" width="25.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="7" width="48.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7913,22 +8030,22 @@
         <v>2019</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>585</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="I2" s="1" t="n">
         <v>4.92</v>
@@ -7942,25 +8059,25 @@
         <v>2020</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>423</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>419</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>850</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>250</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>426</v>
+        <v>429</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>430</v>
       </c>
       <c r="I3" s="1" t="n">
         <v>4.76</v>
@@ -7974,22 +8091,22 @@
         <v>2020</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>218</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>250</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="I4" s="1" t="n">
         <v>4.2</v>
@@ -8003,25 +8120,25 @@
         <v>2021</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>423</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>419</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>850</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>250</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>426</v>
+        <v>429</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>430</v>
       </c>
       <c r="I5" s="1" t="n">
         <v>4.79</v>
@@ -8035,22 +8152,22 @@
         <v>2021</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>218</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>250</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="I6" s="1" t="n">
         <v>4.01</v>
@@ -8064,25 +8181,25 @@
         <v>2022</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>423</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>419</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>850</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>250</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>430</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>426</v>
       </c>
       <c r="I7" s="1" t="n">
         <v>4.33</v>
@@ -8096,22 +8213,22 @@
         <v>2022</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>423</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>419</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>892</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>250</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="I8" s="1" t="n">
         <v>4.29</v>
@@ -8125,22 +8242,22 @@
         <v>2022</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>423</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>419</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>982</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>250</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="I9" s="1" t="n">
         <v>4.34</v>
@@ -8154,25 +8271,25 @@
         <v>2022</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>151</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>250</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>436</v>
+        <v>434</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>440</v>
       </c>
       <c r="I10" s="1" t="n">
         <v>4.95</v>
@@ -8186,22 +8303,22 @@
         <v>2022</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>218</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>250</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="I11" s="1" t="n">
         <v>3.72</v>
@@ -8215,25 +8332,25 @@
         <v>2023</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>151</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>250</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>438</v>
+        <v>434</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>442</v>
       </c>
       <c r="I12" s="1" t="n">
         <v>4.55</v>
@@ -8247,25 +8364,25 @@
         <v>2023</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>251</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>250</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>440</v>
+        <v>434</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>444</v>
       </c>
       <c r="I13" s="1" t="n">
         <v>4.3</v>
@@ -8279,25 +8396,25 @@
         <v>2023</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>423</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>419</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>850</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>250</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="H14" s="12" t="s">
         <v>430</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>426</v>
       </c>
       <c r="I14" s="1" t="n">
         <v>4.31</v>
@@ -8311,25 +8428,25 @@
         <v>2023</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>423</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>419</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>892</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>250</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>441</v>
+        <v>436</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>445</v>
       </c>
       <c r="I15" s="1" t="n">
         <v>4.13</v>
@@ -8343,22 +8460,22 @@
         <v>2023</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>892</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>250</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8366,25 +8483,25 @@
         <v>2024</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>151</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>250</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>438</v>
+        <v>434</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8392,25 +8509,25 @@
         <v>2024</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>251</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>250</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>440</v>
+        <v>434</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update date labels again
</commit_message>
<xml_diff>
--- a/CV.xlsx
+++ b/CV.xlsx
@@ -239,7 +239,7 @@
     <t xml:space="preserve">Center for Statistics and Applications in Forensic Evidence</t>
   </si>
   <si>
-    <t xml:space="preserve">2020-2024</t>
+    <t xml:space="preserve">2020-24</t>
   </si>
   <si>
     <t xml:space="preserve">Assistant Professor</t>
@@ -4898,7 +4898,7 @@
   <dimension ref="A1:AE12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
fix link for cover image
</commit_message>
<xml_diff>
--- a/CV.xlsx
+++ b/CV.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Education" sheetId="1" state="visible" r:id="rId2"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="691">
   <si>
     <t xml:space="preserve">degree</t>
   </si>
@@ -1469,9 +1469,6 @@
   </si>
   <si>
     <t xml:space="preserve">computing, programming, web scraping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/11-asa-computing/#/title-slidehttps://srvanderplas.github.io/2024-Presentations/11-asa-computing/cover.png</t>
   </si>
   <si>
     <t xml:space="preserve">t Seminar</t>
@@ -2526,7 +2523,7 @@
         <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>196</v>
@@ -2535,7 +2532,7 @@
         <v>198</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -2544,22 +2541,22 @@
         <v>20140901</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>522</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>523</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>524</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>525</v>
       </c>
       <c r="H2" s="1"/>
     </row>
@@ -2568,22 +2565,22 @@
         <v>20140501</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>522</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>524</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>525</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -2592,22 +2589,22 @@
         <v>20130801</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>522</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>524</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>525</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -2616,22 +2613,22 @@
         <v>20130501</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>522</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>524</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>525</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -2640,22 +2637,22 @@
         <v>20220117</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>522</v>
-      </c>
       <c r="D6" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>527</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>528</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>283</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2663,22 +2660,22 @@
         <v>20220516</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>522</v>
-      </c>
       <c r="D7" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>527</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>528</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>283</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2686,22 +2683,22 @@
         <v>20230116</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>522</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>283</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2709,22 +2706,22 @@
         <v>20240117</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>522</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>283</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2735,19 +2732,19 @@
         <v>205</v>
       </c>
       <c r="C10" s="10" t="s">
+        <v>529</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>530</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>531</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>532</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>533</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>534</v>
       </c>
     </row>
   </sheetData>
@@ -2776,13 +2773,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>485</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>486</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>38</v>
@@ -2797,7 +2794,7 @@
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I1" s="1"/>
     </row>
@@ -2835,25 +2832,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>538</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>539</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>143</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2873,18 +2870,18 @@
         <v>2019</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>540</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>542</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>543</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>
@@ -2896,15 +2893,15 @@
         <v>2019</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>544</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -2919,13 +2916,13 @@
         <v>2018</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>547</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>541</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2945,13 +2942,13 @@
         <v>2020</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>550</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2971,21 +2968,21 @@
         <v>2020</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>553</v>
-      </c>
       <c r="H6" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>15</v>
@@ -2997,15 +2994,15 @@
         <v>2019</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>555</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>14</v>
@@ -3020,18 +3017,18 @@
         <v>2019</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>557</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>15</v>
@@ -3043,10 +3040,10 @@
         <v>2019</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>560</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3069,10 +3066,10 @@
         <v>129</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>562</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3092,10 +3089,10 @@
         <v>2020</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>564</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3115,13 +3112,13 @@
         <v>2023</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>567</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3141,13 +3138,13 @@
         <v>2023</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>550</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3167,18 +3164,18 @@
         <v>2022</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>569</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>282</v>
@@ -3190,13 +3187,13 @@
         <v>2021</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>573</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3216,10 +3213,10 @@
         <v>2024</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>575</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3239,10 +3236,10 @@
         <v>2023</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>577</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3262,10 +3259,10 @@
         <v>2023</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3285,13 +3282,13 @@
         <v>2024</v>
       </c>
       <c r="F19" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>580</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>581</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3311,10 +3308,10 @@
         <v>0</v>
       </c>
       <c r="F20" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>583</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3334,10 +3331,10 @@
         <v>0</v>
       </c>
       <c r="F21" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>577</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3357,10 +3354,10 @@
         <v>0</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3380,10 +3377,10 @@
         <v>0</v>
       </c>
       <c r="F23" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>585</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3403,10 +3400,10 @@
         <v>0</v>
       </c>
       <c r="F24" s="10" t="s">
+        <v>586</v>
+      </c>
+      <c r="G24" s="10" t="s">
         <v>587</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3417,7 +3414,7 @@
         <v>14</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D25" s="10" t="n">
         <v>2023</v>
@@ -3426,7 +3423,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
   </sheetData>
@@ -3455,16 +3452,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>321</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>591</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>592</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>18</v>
@@ -3472,10 +3469,10 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>593</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>594</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>45007</v>
@@ -3486,7 +3483,7 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>14</v>
@@ -3503,7 +3500,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -3512,7 +3509,7 @@
         <v>44774</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>16</v>
@@ -3520,7 +3517,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>14</v>
@@ -3537,7 +3534,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>14</v>
@@ -3551,13 +3548,13 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>16</v>
@@ -3581,7 +3578,7 @@
   </sheetPr>
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
@@ -3597,19 +3594,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>537</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>538</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>602</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>603</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>143</v>
@@ -3617,7 +3614,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B2" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -3630,18 +3627,18 @@
         <v>2019</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>207</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B3" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -3654,18 +3651,18 @@
         <v>2021</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>608</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B4" s="6" t="b">
         <f aca="false">FALSE()</f>
@@ -3678,16 +3675,16 @@
         <v>2019</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>610</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>611</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3705,21 +3702,21 @@
         <v>2020</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>614</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B6" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -3732,15 +3729,15 @@
         <v>2026</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>616</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B7" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -3753,18 +3750,18 @@
         <v>2022</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>207</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B8" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -3777,10 +3774,10 @@
         <v>2020</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>619</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3798,18 +3795,18 @@
         <v>2021</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B10" s="6" t="b">
         <f aca="false">FALSE()</f>
@@ -3822,18 +3819,18 @@
         <v>2020</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>623</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>624</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B11" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -3846,10 +3843,10 @@
         <v>2024</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3867,21 +3864,21 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>629</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B13" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -3894,13 +3891,13 @@
         <v>2022</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>631</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>632</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>633</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3918,15 +3915,15 @@
         <v>2022</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B15" s="6" t="b">
         <f aca="false">FALSE()</f>
@@ -3939,15 +3936,15 @@
         <v>2021</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B16" s="6" t="b">
         <f aca="false">FALSE()</f>
@@ -3960,18 +3957,18 @@
         <v>2021</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>636</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B17" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -3984,18 +3981,18 @@
         <v>2023</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>207</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B18" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -4008,18 +4005,18 @@
         <v>0</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>639</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>614</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B19" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -4032,18 +4029,18 @@
         <v>2025</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B20" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -4056,18 +4053,18 @@
         <v>2024</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>207</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B21" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -4080,18 +4077,18 @@
         <v>2024</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B22" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -4104,18 +4101,18 @@
         <v>2027</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B23" s="18" t="b">
         <v>1</v>
@@ -4127,16 +4124,16 @@
         <v>0</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="F23" s="0" t="s">
+        <v>644</v>
+      </c>
+      <c r="G23" s="0" t="s">
         <v>645</v>
       </c>
-      <c r="G23" s="0" t="s">
+      <c r="H23" s="0" t="s">
         <v>646</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>647</v>
       </c>
     </row>
   </sheetData>
@@ -4165,10 +4162,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4176,7 +4173,7 @@
         <v>2022</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4184,7 +4181,7 @@
         <v>2019</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4192,7 +4189,7 @@
         <v>2020</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4200,7 +4197,7 @@
         <v>2020</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4208,7 +4205,7 @@
         <v>2020</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4216,7 +4213,7 @@
         <v>2021</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4224,7 +4221,7 @@
         <v>2021</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4232,7 +4229,7 @@
         <v>2021</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4240,7 +4237,7 @@
         <v>2022</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4248,7 +4245,7 @@
         <v>2020</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4256,7 +4253,7 @@
         <v>2021</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4264,7 +4261,7 @@
         <v>2022</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4272,7 +4269,7 @@
         <v>2023</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4280,7 +4277,7 @@
         <v>2022</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4288,7 +4285,7 @@
         <v>2023</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4296,7 +4293,7 @@
         <v>2023</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4304,7 +4301,7 @@
         <v>2023</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4312,7 +4309,7 @@
         <v>2023</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
   </sheetData>
@@ -4344,22 +4341,22 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>658</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>659</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>143</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>660</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>661</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4374,10 +4371,10 @@
         <v>2023</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>663</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4392,10 +4389,10 @@
         <v>2023</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>665</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4410,10 +4407,10 @@
         <v>2022</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>667</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4428,7 +4425,7 @@
         <v>2020</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4443,10 +4440,10 @@
         <v>2020</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>670</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>671</v>
       </c>
     </row>
   </sheetData>
@@ -4481,10 +4478,10 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>658</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>659</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>143</v>
@@ -4493,13 +4490,13 @@
         <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>660</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>661</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>662</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -4511,7 +4508,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C2" s="12" t="n">
         <v>2023</v>
@@ -4520,13 +4517,13 @@
         <v>2023</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>673</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>674</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>675</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -4539,7 +4536,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C3" s="12" t="n">
         <v>2022</v>
@@ -4548,13 +4545,13 @@
         <v>2022</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>676</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>677</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>678</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -4567,7 +4564,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C4" s="12" t="n">
         <v>2022</v>
@@ -4576,13 +4573,13 @@
         <v>2022</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>679</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>680</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -4595,7 +4592,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C5" s="12" t="n">
         <v>2022</v>
@@ -4604,13 +4601,13 @@
         <v>2022</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>681</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>682</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -4623,7 +4620,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C6" s="12" t="n">
         <v>2021</v>
@@ -4632,13 +4629,13 @@
         <v>2021</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -4652,7 +4649,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C7" s="12" t="n">
         <v>2021</v>
@@ -4661,13 +4658,13 @@
         <v>2021</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>685</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>686</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>687</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -4681,7 +4678,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C8" s="12" t="n">
         <v>2021</v>
@@ -4693,10 +4690,10 @@
         <v>351</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -4710,7 +4707,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C9" s="12" t="n">
         <v>2020</v>
@@ -4719,16 +4716,16 @@
         <v>2020</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>689</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>686</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>690</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>691</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -6802,10 +6799,10 @@
   </sheetPr>
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L48" activeCellId="0" sqref="L48"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="L47" activeCellId="0" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8482,9 +8479,7 @@
       <c r="K47" s="10" t="s">
         <v>475</v>
       </c>
-      <c r="L47" s="10" t="s">
-        <v>476</v>
-      </c>
+      <c r="L47" s="10"/>
     </row>
     <row r="48" customFormat="false" ht="57.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="8" t="n">
@@ -8500,31 +8495,30 @@
         <v>321</v>
       </c>
       <c r="E48" s="10" t="s">
+        <v>476</v>
+      </c>
+      <c r="F48" s="15" t="s">
         <v>477</v>
-      </c>
-      <c r="F48" s="15" t="s">
-        <v>478</v>
       </c>
       <c r="H48" s="10" t="s">
         <v>283</v>
       </c>
       <c r="I48" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="J48" s="10" t="s">
         <v>479</v>
-      </c>
-      <c r="J48" s="10" t="s">
-        <v>480</v>
       </c>
       <c r="K48" s="10" t="s">
         <v>455</v>
       </c>
       <c r="L48" s="10" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L46" r:id="rId1" display="https://srvanderplas.github.io/2024-Presentations/08-JSM/index_files/figure-revealjs/unnamed-chunk-15-1.png"/>
-    <hyperlink ref="L47" r:id="rId2" location="/title-slidehttps://srvanderplas.github.io/2024-Presentations/11-asa-computing/cover.png" display="https://srvanderplas.github.io/2024-Presentations/11-asa-computing/#/title-slidehttps://srvanderplas.github.io/2024-Presentations/11-asa-computing/cover.png"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -8558,34 +8552,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>485</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>486</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>489</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8593,22 +8587,22 @@
         <v>2019</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>492</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>585</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>494</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>495</v>
       </c>
       <c r="I2" s="1" t="n">
         <v>4.92</v>
@@ -8622,25 +8616,25 @@
         <v>2020</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>850</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="H3" s="14" t="s">
         <v>498</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>499</v>
       </c>
       <c r="I3" s="1" t="n">
         <v>4.76</v>
@@ -8654,22 +8648,22 @@
         <v>2020</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>492</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>218</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I4" s="1" t="n">
         <v>4.2</v>
@@ -8683,25 +8677,25 @@
         <v>2021</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>850</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="H5" s="14" t="s">
         <v>498</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>499</v>
       </c>
       <c r="I5" s="1" t="n">
         <v>4.79</v>
@@ -8715,22 +8709,22 @@
         <v>2021</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>492</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>218</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I6" s="1" t="n">
         <v>4.01</v>
@@ -8744,25 +8738,25 @@
         <v>2022</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>850</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I7" s="1" t="n">
         <v>4.33</v>
@@ -8776,22 +8770,22 @@
         <v>2022</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>892</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I8" s="1" t="n">
         <v>4.29</v>
@@ -8805,22 +8799,22 @@
         <v>2022</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>982</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I9" s="1" t="n">
         <v>4.34</v>
@@ -8834,25 +8828,25 @@
         <v>2022</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>492</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>151</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="I10" s="1" t="n">
         <v>4.95</v>
@@ -8866,22 +8860,22 @@
         <v>2022</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>492</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>218</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="I11" s="1" t="n">
         <v>3.72</v>
@@ -8895,25 +8889,25 @@
         <v>2023</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>492</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>151</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="I12" s="1" t="n">
         <v>4.55</v>
@@ -8927,25 +8921,25 @@
         <v>2023</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>492</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>251</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I13" s="1" t="n">
         <v>4.3</v>
@@ -8959,25 +8953,25 @@
         <v>2023</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>850</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I14" s="1" t="n">
         <v>4.31</v>
@@ -8991,25 +8985,25 @@
         <v>2023</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>892</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="I15" s="1" t="n">
         <v>4.13</v>
@@ -9023,22 +9017,22 @@
         <v>2023</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>492</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>892</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9046,25 +9040,25 @@
         <v>2024</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>492</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>151</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9072,25 +9066,25 @@
         <v>2024</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>492</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>251</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9098,25 +9092,25 @@
         <v>2024</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D19" s="10" t="n">
         <v>892</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -9126,22 +9120,22 @@
         <v>2024</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D20" s="10" t="n">
         <v>992</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>452</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update link to cover image
</commit_message>
<xml_diff>
--- a/CV.xlsx
+++ b/CV.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="692">
   <si>
     <t xml:space="preserve">degree</t>
   </si>
@@ -1469,6 +1469,9 @@
   </si>
   <si>
     <t xml:space="preserve">computing, programming, web scraping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/11-asa-computing/cover.png</t>
   </si>
   <si>
     <t xml:space="preserve">t Seminar</t>
@@ -2128,7 +2131,7 @@
     <numFmt numFmtId="168" formatCode="yyyy\-mm"/>
     <numFmt numFmtId="169" formatCode="yyyy\-m"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2165,6 +2168,12 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2215,7 +2224,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2280,6 +2289,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2523,7 +2536,7 @@
         <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>196</v>
@@ -2532,7 +2545,7 @@
         <v>198</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -2541,22 +2554,22 @@
         <v>20140901</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="H2" s="1"/>
     </row>
@@ -2565,22 +2578,22 @@
         <v>20140501</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -2589,22 +2602,22 @@
         <v>20130801</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -2613,22 +2626,22 @@
         <v>20130501</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -2637,22 +2650,22 @@
         <v>20220117</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>283</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2660,22 +2673,22 @@
         <v>20220516</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>283</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2683,22 +2696,22 @@
         <v>20230116</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>283</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2706,22 +2719,22 @@
         <v>20240117</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>283</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2732,19 +2745,19 @@
         <v>205</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
   </sheetData>
@@ -2773,13 +2786,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>38</v>
@@ -2794,7 +2807,7 @@
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="I1" s="1"/>
     </row>
@@ -2832,25 +2845,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>143</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2870,18 +2883,18 @@
         <v>2019</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>
@@ -2893,15 +2906,15 @@
         <v>2019</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -2916,13 +2929,13 @@
         <v>2018</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2942,13 +2955,13 @@
         <v>2020</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2968,21 +2981,21 @@
         <v>2020</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>551</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>15</v>
@@ -2994,15 +3007,15 @@
         <v>2019</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>14</v>
@@ -3017,18 +3030,18 @@
         <v>2019</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>15</v>
@@ -3040,10 +3053,10 @@
         <v>2019</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3066,10 +3079,10 @@
         <v>129</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3089,10 +3102,10 @@
         <v>2020</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3112,13 +3125,13 @@
         <v>2023</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3138,13 +3151,13 @@
         <v>2023</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3164,18 +3177,18 @@
         <v>2022</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>282</v>
@@ -3187,13 +3200,13 @@
         <v>2021</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3213,10 +3226,10 @@
         <v>2024</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3236,10 +3249,10 @@
         <v>2023</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3259,10 +3272,10 @@
         <v>2023</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3282,13 +3295,13 @@
         <v>2024</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3308,10 +3321,10 @@
         <v>0</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3331,10 +3344,10 @@
         <v>0</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3354,10 +3367,10 @@
         <v>0</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3377,10 +3390,10 @@
         <v>0</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3400,10 +3413,10 @@
         <v>0</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3414,7 +3427,7 @@
         <v>14</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="D25" s="10" t="n">
         <v>2023</v>
@@ -3423,7 +3436,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
   </sheetData>
@@ -3452,16 +3465,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>321</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>18</v>
@@ -3469,10 +3482,10 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>45007</v>
@@ -3483,15 +3496,15 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="16" t="n">
+      <c r="C3" s="17" t="n">
         <v>44774</v>
       </c>
-      <c r="D3" s="16" t="n">
+      <c r="D3" s="17" t="n">
         <v>45047</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -3500,16 +3513,16 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="16" t="n">
+      <c r="C4" s="17" t="n">
         <v>44774</v>
       </c>
-      <c r="D4" s="16" t="s">
-        <v>596</v>
+      <c r="D4" s="17" t="s">
+        <v>597</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>16</v>
@@ -3517,15 +3530,15 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="17" t="n">
+      <c r="C5" s="18" t="n">
         <v>44835</v>
       </c>
-      <c r="D5" s="16" t="n">
+      <c r="D5" s="17" t="n">
         <v>45047</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -3534,12 +3547,12 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="16" t="n">
+      <c r="C6" s="17" t="n">
         <v>44409</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -3548,13 +3561,13 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>16</v>
@@ -3594,19 +3607,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>143</v>
@@ -3614,7 +3627,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B2" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -3627,18 +3640,18 @@
         <v>2019</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>207</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B3" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -3651,18 +3664,18 @@
         <v>2021</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>606</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>607</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B4" s="6" t="b">
         <f aca="false">FALSE()</f>
@@ -3675,16 +3688,16 @@
         <v>2019</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3702,21 +3715,21 @@
         <v>2020</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B6" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -3729,15 +3742,15 @@
         <v>2026</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B7" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -3750,18 +3763,18 @@
         <v>2022</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>207</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B8" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -3774,10 +3787,10 @@
         <v>2020</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3795,18 +3808,18 @@
         <v>2021</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="B10" s="6" t="b">
         <f aca="false">FALSE()</f>
@@ -3819,18 +3832,18 @@
         <v>2020</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B11" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -3843,10 +3856,10 @@
         <v>2024</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3864,21 +3877,21 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="B13" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -3891,13 +3904,13 @@
         <v>2022</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3915,15 +3928,15 @@
         <v>2022</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="B15" s="6" t="b">
         <f aca="false">FALSE()</f>
@@ -3936,15 +3949,15 @@
         <v>2021</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="B16" s="6" t="b">
         <f aca="false">FALSE()</f>
@@ -3957,18 +3970,18 @@
         <v>2021</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B17" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -3981,18 +3994,18 @@
         <v>2023</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>207</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="B18" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -4005,18 +4018,18 @@
         <v>0</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B19" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -4029,18 +4042,18 @@
         <v>2025</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>606</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>640</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B20" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -4053,18 +4066,18 @@
         <v>2024</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>207</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="B21" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -4077,18 +4090,18 @@
         <v>2024</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="B22" s="6" t="b">
         <f aca="false">TRUE()</f>
@@ -4101,20 +4114,20 @@
         <v>2027</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>603</v>
-      </c>
-      <c r="B23" s="18" t="b">
+        <v>604</v>
+      </c>
+      <c r="B23" s="19" t="b">
         <v>1</v>
       </c>
       <c r="C23" s="0" t="n">
@@ -4124,16 +4137,16 @@
         <v>0</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
   </sheetData>
@@ -4162,10 +4175,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4173,7 +4186,7 @@
         <v>2022</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4181,7 +4194,7 @@
         <v>2019</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4189,7 +4202,7 @@
         <v>2020</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4197,7 +4210,7 @@
         <v>2020</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4205,7 +4218,7 @@
         <v>2020</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4213,7 +4226,7 @@
         <v>2021</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4221,7 +4234,7 @@
         <v>2021</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4229,7 +4242,7 @@
         <v>2021</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4237,7 +4250,7 @@
         <v>2022</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4245,7 +4258,7 @@
         <v>2020</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4253,7 +4266,7 @@
         <v>2021</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4261,7 +4274,7 @@
         <v>2022</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4269,7 +4282,7 @@
         <v>2023</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4277,7 +4290,7 @@
         <v>2022</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4285,7 +4298,7 @@
         <v>2023</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4293,7 +4306,7 @@
         <v>2023</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4301,7 +4314,7 @@
         <v>2023</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4309,7 +4322,7 @@
         <v>2023</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
   </sheetData>
@@ -4341,22 +4354,22 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>143</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4371,10 +4384,10 @@
         <v>2023</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4389,10 +4402,10 @@
         <v>2023</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4407,10 +4420,10 @@
         <v>2022</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4425,7 +4438,7 @@
         <v>2020</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4440,10 +4453,10 @@
         <v>2020</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
   </sheetData>
@@ -4478,10 +4491,10 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>143</v>
@@ -4490,13 +4503,13 @@
         <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -4508,7 +4521,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="C2" s="12" t="n">
         <v>2023</v>
@@ -4517,13 +4530,13 @@
         <v>2023</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -4536,7 +4549,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="C3" s="12" t="n">
         <v>2022</v>
@@ -4545,13 +4558,13 @@
         <v>2022</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -4564,7 +4577,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="C4" s="12" t="n">
         <v>2022</v>
@@ -4573,13 +4586,13 @@
         <v>2022</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -4592,7 +4605,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="C5" s="12" t="n">
         <v>2022</v>
@@ -4601,13 +4614,13 @@
         <v>2022</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -4620,7 +4633,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="C6" s="12" t="n">
         <v>2021</v>
@@ -4629,13 +4642,13 @@
         <v>2021</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -4649,7 +4662,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="C7" s="12" t="n">
         <v>2021</v>
@@ -4658,13 +4671,13 @@
         <v>2021</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -4678,7 +4691,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="C8" s="12" t="n">
         <v>2021</v>
@@ -4690,10 +4703,10 @@
         <v>351</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -4707,7 +4720,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="C9" s="12" t="n">
         <v>2020</v>
@@ -4716,16 +4729,16 @@
         <v>2020</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -8479,7 +8492,9 @@
       <c r="K47" s="10" t="s">
         <v>475</v>
       </c>
-      <c r="L47" s="10"/>
+      <c r="L47" s="16" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="57.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="8" t="n">
@@ -8495,30 +8510,31 @@
         <v>321</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="H48" s="10" t="s">
         <v>283</v>
       </c>
       <c r="I48" s="10" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="K48" s="10" t="s">
         <v>455</v>
       </c>
       <c r="L48" s="10" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L46" r:id="rId1" display="https://srvanderplas.github.io/2024-Presentations/08-JSM/index_files/figure-revealjs/unnamed-chunk-15-1.png"/>
+    <hyperlink ref="L47" r:id="rId2" display="https://srvanderplas.github.io/2024-Presentations/11-asa-computing/cover.png"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -8552,34 +8568,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8587,22 +8603,22 @@
         <v>2019</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>585</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="I2" s="1" t="n">
         <v>4.92</v>
@@ -8616,25 +8632,25 @@
         <v>2020</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>850</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="I3" s="1" t="n">
         <v>4.76</v>
@@ -8648,22 +8664,22 @@
         <v>2020</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>218</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="I4" s="1" t="n">
         <v>4.2</v>
@@ -8677,25 +8693,25 @@
         <v>2021</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>850</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="I5" s="1" t="n">
         <v>4.79</v>
@@ -8709,22 +8725,22 @@
         <v>2021</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>218</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="I6" s="1" t="n">
         <v>4.01</v>
@@ -8738,25 +8754,25 @@
         <v>2022</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>850</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="I7" s="1" t="n">
         <v>4.33</v>
@@ -8770,22 +8786,22 @@
         <v>2022</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>892</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="I8" s="1" t="n">
         <v>4.29</v>
@@ -8799,22 +8815,22 @@
         <v>2022</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>982</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="I9" s="1" t="n">
         <v>4.34</v>
@@ -8828,25 +8844,25 @@
         <v>2022</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>151</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="I10" s="1" t="n">
         <v>4.95</v>
@@ -8860,22 +8876,22 @@
         <v>2022</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>218</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="I11" s="1" t="n">
         <v>3.72</v>
@@ -8889,25 +8905,25 @@
         <v>2023</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>151</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="I12" s="1" t="n">
         <v>4.55</v>
@@ -8921,25 +8937,25 @@
         <v>2023</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>251</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="I13" s="1" t="n">
         <v>4.3</v>
@@ -8953,25 +8969,25 @@
         <v>2023</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>850</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="I14" s="1" t="n">
         <v>4.31</v>
@@ -8985,25 +9001,25 @@
         <v>2023</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>892</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="I15" s="1" t="n">
         <v>4.13</v>
@@ -9017,22 +9033,22 @@
         <v>2023</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>892</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9040,25 +9056,25 @@
         <v>2024</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>151</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9066,25 +9082,25 @@
         <v>2024</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>251</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9092,25 +9108,25 @@
         <v>2024</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D19" s="10" t="n">
         <v>892</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -9120,22 +9136,22 @@
         <v>2024</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D20" s="10" t="n">
         <v>992</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>452</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix cv data at source
</commit_message>
<xml_diff>
--- a/CV.xlsx
+++ b/CV.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Education" sheetId="1" state="visible" r:id="rId2"/>
@@ -1385,7 +1385,7 @@
     <t xml:space="preserve">Chicago, IL (Online)</t>
   </si>
   <si>
-    <t xml:space="preserve">During COVID, people all over the world were consulting time-series charts on a daily basis and using these charts to make decisions. Discussions broke out among data visualization and scientific communication experts, debating the relative merits of log and linear scales, but there was relatively little research about how people perceive and use visualizations of exponential data, with linear or transformed scales. In this talk, I’ll discuss the study we undertook to address the lack of research in this area, and how the results speak not only to the importance of additional graphical testing, but also to the trade offs between different levels of user engagement with visualizations.</t>
+    <t xml:space="preserve">During COVID, people all over the world were consulting time-series charts on a daily basis and using these charts to make decisions. Discussions broke out among data visualization and scientific communication experts, debating the relative merits of log and linear scales, but there was relatively little research about how people perceive and use visualizations of exponential data, with linear or transformed scales. In this talk, I'll discuss the study we undertook to address the lack of research in this area, and how the results speak not only to the importance of additional graphical testing, but also to the trade offs between different levels of user engagement with visualizations.</t>
   </si>
   <si>
     <t xml:space="preserve">Creating Good Graphics</t>
@@ -1394,220 +1394,220 @@
     <t xml:space="preserve">UNL REU seminar</t>
   </si>
   <si>
+    <t xml:space="preserve">Let's talk about how to create good charts and graphics!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/06-REU-graphics/#/title-slide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">graphics, visualization, design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/06-REU-graphics/3d-stacked-pie-chart.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Escaping Flatland: Graphics, Dimensionality, and Human Perception</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human Computer Interaction International</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Washington DC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Almost 40 years ago, Cleveland &amp; McGill published the first of 3 papers detailing experiments assessing the accuracy of numerical perception using different types of charts. This study is often cited as a reason to avoid the use of extraneous dimensions in data visualization: 2D bar charts produced more accurate estimates than 3D bar charts; in addition, lines (length) produced more accurate estimates than circles (area). Graphics have changed fairly significantly in the last 40 years: where we once had fixed 3D perspective charts, we now can rotate 3D renderings in digital space and even 3D print our charts to examine physically. Many optical illusions result from perceptual mismatches of 3D visual heuristics and 2D, planar, data representations; more realistic renderings available with modern tools might change the outcome of the Cleveland &amp; McGill comparison of 2D vs. 3D accuracy. In this paper, we present several experiments which replicate the bar chart portion of Cleveland &amp; McGill's original study, comparing 2D, 3D fixed perspective, 3D rendered, and 3D printed charts. We discuss the findings and the importance of replicating classic experiments using modern technology, as well as the benefits of incorporating hands-on research in introductory classes as experiential learning activities.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/07-HCII/#/title-slide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teaching, graphics, user-study, 3d, visualization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/07-HCII/cover.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Plot is Worth a Thousand Tests: Assessing Residual Diagnostics with the Lineup Protocol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weihao (Patrick) Li, Di Cook, Emi Tanaka, Klaus Ackermann, Susan Vanderplas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portland, Or</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regression experts consistently recommend plotting residuals for model diagnosis, despite the availability of many numerical hypothesis test procedures designed to use residuals to assess problems with a model fit. Here we provide evidence for why this is good advice using data from a visual inference experiment. We show how conventional tests are too sensitive, which means that too often the conclusion would be that the model fit is inadequate. The experiment uses the lineup protocol which puts a residual plot in the context of null plots. This helps generate reliable and consistent reading of residual plots for better model diagnosis. It can also help in an obverse situation where a conventional test would fail to detect a problem with a model due to contaminated data. The lineup protocol also detects a range of departures from good residuals simultaneously. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/08-JSM/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visualization, graphics, visual inference, user study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/08-JSM/index_files/figure-revealjs/unnamed-chunk-15-1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Scraping Olympics: Python</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statistical Computing Section Mini-Symposium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A comparison of Python, Julia, and R for web-scraping Olympic athlete names, events, and birthdays. I represented python. See the full narrative here: https://srvanderplas.github.io/2024-data-jamboree-python/python-narrative.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/11-asa-computing/#/title-slide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">computing, programming, web scraping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/11-asa-computing/cover.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creating Effective Graphics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Undergraduate Creative Activities and Research Experience</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How do we create effective charts and graphs for scientific presentations? What are the elements of effective charts and graphics? Which charts should be used for different types of data? How do we make charts that are "presentation ready"? In this workshop, we'll do a quick run-through of guidelines for good charts and graphics, and then discuss how to use different scientific tools to create charts and graphics effectively. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/11-fyre-graphics/#/title-slide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/11-fyre-graphics/data-to-vis-flowchart.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hidden Multiple Comparisons Increase Forensic Error Rates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENAR Spring Meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Orleans, Louisiana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When wires are cut, the tool produces striations on the cut surface; as in other forms of forensic analysis, these striation marks are used to connect the evidence to the source that created them. The practice of comparing two wire cut surfaces introduces complexities not present in better-investigated forensic examination of toolmarks such as those observed on bullets, as wire comparisons inherently require multiple distinct comparisons, increasing the error rate. We call attention to this multiple comparison problem in wire examination, and relate it to other situations in forensics that involve multiple comparisons, such as database searches.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://srvanderplas.github.io/2025-Presentations/03-ENAR/#/title-slide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">forensics, error rates, wires, probability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://srvanderplas.github.io/2025-Presentations/03-ENAR/wire_cutter.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">semester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">course_prefix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">course_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">course_title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">course_materials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eval_mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eval_median</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Technologies for Statistical Analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iowa State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Co-taught with Heike Hofmann</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computing Tools for Statisticians</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hybrid, flipped, synchronous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://unl-statistics.github.io/stat850/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to Statistics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initially in person synchronous, then online asynchronous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Online asynchronous.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flipped synchronous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Writing in Statistics/TA Prep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In person synchronous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advanced Inference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Co-taught with Bertrand Clarke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to Statistical Computing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://unl-statistics.github.io/stat151/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Online asynchronous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Wrangling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://unl-statistics.github.io/stat251/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://unl-statistics.github.io/stat892-TA-prep/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Co-taught with ISU Stat 585, Hybrid synchronous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Special Topics in Data Visualization</t>
+  </si>
+  <si>
     <t xml:space="preserve">University of Nebraska – Lincoln</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Let's talk about how to create good charts and graphics!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/06-REU-graphics/#/title-slide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">graphics, visualization, design</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/06-REU-graphics/3d-stacked-pie-chart.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Escaping Flatland: Graphics, Dimensionality, and Human Perception</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Human Computer Interaction International</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Washington DC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Almost 40 years ago, Cleveland &amp; McGill published the first of 3 papers detailing experiments assessing the accuracy of numerical perception using different types of charts. This study is often cited as a reason to avoid the use of extraneous dimensions in data visualization: 2D bar charts produced more accurate estimates than 3D bar charts; in addition, lines (length) produced more accurate estimates than circles (area). Graphics have changed fairly significantly in the last 40 years: where we once had fixed 3D perspective charts, we now can rotate 3D renderings in digital space and even 3D print our charts to examine physically. Many optical illusions result from perceptual mismatches of 3D visual heuristics and 2D, planar, data representations; more realistic renderings available with modern tools might change the outcome of the Cleveland &amp; McGill comparison of 2D vs. 3D accuracy. In this paper, we present several experiments which replicate the bar chart portion of Cleveland &amp; McGill's original study, comparing 2D, 3D fixed perspective, 3D rendered, and 3D printed charts. We discuss the findings and the importance of replicating classic experiments using modern technology, as well as the benefits of incorporating hands-on research in introductory classes as experiential learning activities.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/07-HCII/#/title-slide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">teaching, graphics, user-study, 3d, visualization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/07-HCII/cover.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A Plot is Worth a Thousand Tests: Assessing Residual Diagnostics with the Lineup Protocol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weihao (Patrick) Li, Di Cook, Emi Tanaka, Klaus Ackermann, Susan Vanderplas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Portland, Or</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regression experts consistently recommend plotting residuals for model diagnosis, despite the availability of many numerical hypothesis test procedures designed to use residuals to assess problems with a model fit. Here we provide evidence for why this is good advice using data from a visual inference experiment. We show how conventional tests are too sensitive, which means that too often the conclusion would be that the model fit is inadequate. The experiment uses the lineup protocol which puts a residual plot in the context of null plots. This helps generate reliable and consistent reading of residual plots for better model diagnosis. It can also help in an obverse situation where a conventional test would fail to detect a problem with a model due to contaminated data. The lineup protocol also detects a range of departures from good residuals simultaneously. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/08-JSM/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">visualization, graphics, visual inference, user study</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/08-JSM/index_files/figure-revealjs/unnamed-chunk-15-1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Web Scraping Olympics: Python</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Statistical Computing Section Mini-Symposium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A comparison of Python, Julia, and R for web-scraping Olympic athlete names, events, and birthdays. I represented python. See the full narrative here: https://srvanderplas.github.io/2024-data-jamboree-python/python-narrative.html </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/11-asa-computing/#/title-slide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">computing, programming, web scraping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/11-asa-computing/cover.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creating Effective Graphics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Undergraduate Creative Activities and Research Experience</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How do we create effective charts and graphs for scientific presentations? What are the elements of effective charts and graphics? Which charts should be used for different types of data? How do we make charts that are "presentation ready"? In this workshop, we'll do a quick run-through of guidelines for good charts and graphics, and then discuss how to use different scientific tools to create charts and graphics effectively. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/11-fyre-graphics/#/title-slide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://srvanderplas.github.io/2024-Presentations/11-fyre-graphics/data-to-vis-flowchart.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hidden Multiple Comparisons Increase Forensic Error Rates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENAR Spring Meeting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Orleans, Louisiana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When wires are cut, the tool produces striations on the cut surface; as in other forms of forensic analysis, these striation marks are used to connect the evidence to the source that created them. The practice of comparing two wire cut surfaces introduces complexities not present in better-investigated forensic examination of toolmarks such as those observed on bullets, as wire comparisons inherently require multiple distinct comparisons, increasing the error rate. We call attention to this multiple comparison problem in wire examination, and relate it to other situations in forensics that involve multiple comparisons, such as database searches.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://srvanderplas.github.io/2025-Presentations/03-ENAR/#/title-slide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">forensics, error rates, wires, probability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://srvanderplas.github.io/2025-Presentations/03-ENAR/wire_cutter.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">semester</t>
-  </si>
-  <si>
-    <t xml:space="preserve">course_prefix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">course_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">course_title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">note</t>
-  </si>
-  <si>
-    <t xml:space="preserve">course_materials</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eval_mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eval_median</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spring</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Technologies for Statistical Analysis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iowa State</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Co-taught with Heike Hofmann</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computing Tools for Statisticians</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hybrid, flipped, synchronous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://unl-statistics.github.io/stat850/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduction to Statistics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initially in person synchronous, then online asynchronous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Online asynchronous.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flipped synchronous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Writing in Statistics/TA Prep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In person synchronous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Advanced Inference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Co-taught with Bertrand Clarke</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduction to Statistical Computing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://unl-statistics.github.io/stat151/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Online asynchronous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Wrangling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://unl-statistics.github.io/stat251/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://unl-statistics.github.io/stat892-TA-prep/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Co-taught with ISU Stat 585, Hybrid synchronous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Special Topics in Data Visualization</t>
   </si>
   <si>
     <t xml:space="preserve">Technical Skills for Statisticians</t>
@@ -2817,13 +2817,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>492</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>493</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>38</v>
@@ -2844,13 +2844,13 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B2" s="9" t="n">
         <v>151</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>283</v>
@@ -2871,13 +2871,13 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B3" s="9" t="n">
         <v>251</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>283</v>
@@ -2898,7 +2898,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B4" s="9" t="n">
         <v>850</v>
@@ -2925,7 +2925,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B5" s="9" t="n">
         <v>349</v>
@@ -2968,7 +2968,7 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
@@ -3002,7 +3002,7 @@
         <v>143</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3520,7 +3520,7 @@
         <v>14</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>452</v>
+        <v>523</v>
       </c>
       <c r="D23" s="9" t="n">
         <v>2024</v>
@@ -4420,7 +4420,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>668</v>
@@ -7047,10 +7047,10 @@
   </sheetPr>
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M53" activeCellId="0" sqref="M53"/>
+      <selection pane="bottomLeft" activeCell="K22" activeCellId="0" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8605,22 +8605,22 @@
         <v>451</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>452</v>
+        <v>282</v>
       </c>
       <c r="H44" s="9" t="s">
         <v>283</v>
       </c>
       <c r="I44" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="J44" s="9" t="s">
         <v>453</v>
       </c>
-      <c r="J44" s="9" t="s">
+      <c r="K44" s="9" t="s">
         <v>454</v>
       </c>
-      <c r="K44" s="9" t="s">
+      <c r="L44" s="9" t="s">
         <v>455</v>
-      </c>
-      <c r="L44" s="9" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8631,7 +8631,7 @@
         <v>223</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D45" s="9" t="s">
         <v>218</v>
@@ -8640,22 +8640,22 @@
         <v>205</v>
       </c>
       <c r="F45" s="9" t="s">
+        <v>457</v>
+      </c>
+      <c r="H45" s="9" t="s">
         <v>458</v>
       </c>
-      <c r="H45" s="9" t="s">
+      <c r="I45" s="9" t="s">
         <v>459</v>
       </c>
-      <c r="I45" s="9" t="s">
+      <c r="J45" s="9" t="s">
         <v>460</v>
       </c>
-      <c r="J45" s="9" t="s">
+      <c r="K45" s="9" t="s">
         <v>461</v>
       </c>
-      <c r="K45" s="9" t="s">
+      <c r="L45" s="9" t="s">
         <v>462</v>
-      </c>
-      <c r="L45" s="9" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8666,10 +8666,10 @@
         <v>223</v>
       </c>
       <c r="C46" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="D46" s="9" t="s">
         <v>464</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>465</v>
       </c>
       <c r="E46" s="9" t="s">
         <v>205</v>
@@ -8681,19 +8681,19 @@
         <v>207</v>
       </c>
       <c r="H46" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="I46" s="9" t="s">
         <v>466</v>
       </c>
-      <c r="I46" s="9" t="s">
+      <c r="J46" s="9" t="s">
         <v>467</v>
       </c>
-      <c r="J46" s="9" t="s">
+      <c r="K46" s="9" t="s">
         <v>468</v>
       </c>
-      <c r="K46" s="9" t="s">
+      <c r="L46" s="9" t="s">
         <v>469</v>
-      </c>
-      <c r="L46" s="9" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8704,7 +8704,7 @@
         <v>223</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D47" s="9" t="s">
         <v>218</v>
@@ -8713,22 +8713,22 @@
         <v>351</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H47" s="9" t="s">
         <v>290</v>
       </c>
       <c r="I47" s="9" t="s">
+        <v>472</v>
+      </c>
+      <c r="J47" s="9" t="s">
         <v>473</v>
       </c>
-      <c r="J47" s="9" t="s">
+      <c r="K47" s="9" t="s">
         <v>474</v>
       </c>
-      <c r="K47" s="9" t="s">
+      <c r="L47" s="9" t="s">
         <v>475</v>
-      </c>
-      <c r="L47" s="9" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="18.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8739,7 +8739,7 @@
         <v>279</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D48" s="9" t="s">
         <v>218</v>
@@ -8748,22 +8748,22 @@
         <v>281</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="H48" s="9" t="s">
         <v>283</v>
       </c>
       <c r="I48" s="9" t="s">
+        <v>478</v>
+      </c>
+      <c r="J48" s="9" t="s">
         <v>479</v>
       </c>
-      <c r="J48" s="9" t="s">
+      <c r="K48" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="L48" s="9" t="s">
         <v>480</v>
-      </c>
-      <c r="K48" s="9" t="s">
-        <v>455</v>
-      </c>
-      <c r="L48" s="9" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8774,7 +8774,7 @@
         <v>223</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D49" s="9" t="s">
         <v>218</v>
@@ -8783,22 +8783,22 @@
         <v>205</v>
       </c>
       <c r="F49" s="9" t="s">
+        <v>482</v>
+      </c>
+      <c r="H49" s="9" t="s">
         <v>483</v>
       </c>
-      <c r="H49" s="9" t="s">
+      <c r="I49" s="9" t="s">
         <v>484</v>
       </c>
-      <c r="I49" s="9" t="s">
+      <c r="J49" s="9" t="s">
         <v>485</v>
       </c>
-      <c r="J49" s="9" t="s">
+      <c r="K49" s="9" t="s">
         <v>486</v>
       </c>
-      <c r="K49" s="9" t="s">
+      <c r="M49" s="9" t="s">
         <v>487</v>
-      </c>
-      <c r="M49" s="9" t="s">
-        <v>488</v>
       </c>
     </row>
   </sheetData>
@@ -8838,34 +8838,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>492</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>493</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>496</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8873,22 +8873,22 @@
         <v>2019</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>498</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>499</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>585</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>501</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>502</v>
       </c>
       <c r="I2" s="1" t="n">
         <v>4.92</v>
@@ -8902,25 +8902,25 @@
         <v>2020</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>850</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>505</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>506</v>
       </c>
       <c r="I3" s="1" t="n">
         <v>4.76</v>
@@ -8934,22 +8934,22 @@
         <v>2020</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>498</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>499</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>218</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I4" s="1" t="n">
         <v>4.2</v>
@@ -8963,25 +8963,25 @@
         <v>2021</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>850</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="H5" s="12" t="s">
         <v>505</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>506</v>
       </c>
       <c r="I5" s="1" t="n">
         <v>4.79</v>
@@ -8995,22 +8995,22 @@
         <v>2021</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>498</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>499</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>218</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="I6" s="1" t="n">
         <v>4.01</v>
@@ -9024,25 +9024,25 @@
         <v>2022</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>850</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I7" s="1" t="n">
         <v>4.33</v>
@@ -9056,22 +9056,22 @@
         <v>2022</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>892</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I8" s="1" t="n">
         <v>4.29</v>
@@ -9085,22 +9085,22 @@
         <v>2022</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>982</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="I9" s="1" t="n">
         <v>4.34</v>
@@ -9114,25 +9114,25 @@
         <v>2022</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>498</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>499</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>151</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="I10" s="1" t="n">
         <v>4.95</v>
@@ -9146,22 +9146,22 @@
         <v>2022</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>498</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>499</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>218</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I11" s="1" t="n">
         <v>3.72</v>
@@ -9175,25 +9175,25 @@
         <v>2023</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>498</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>499</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>151</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="I12" s="1" t="n">
         <v>4.55</v>
@@ -9207,25 +9207,25 @@
         <v>2023</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>498</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>499</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>251</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="I13" s="1" t="n">
         <v>4.3</v>
@@ -9239,25 +9239,25 @@
         <v>2023</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>850</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I14" s="1" t="n">
         <v>4.31</v>
@@ -9271,25 +9271,25 @@
         <v>2023</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>892</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I15" s="1" t="n">
         <v>4.13</v>
@@ -9303,22 +9303,22 @@
         <v>2023</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>498</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>499</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>892</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9326,25 +9326,25 @@
         <v>2024</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>498</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>499</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>151</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9352,25 +9352,25 @@
         <v>2024</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>498</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>499</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>251</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9378,25 +9378,25 @@
         <v>2024</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D19" s="9" t="n">
         <v>892</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>282</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -9406,22 +9406,22 @@
         <v>2024</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D20" s="9" t="n">
         <v>992</v>
       </c>
       <c r="E20" s="9" t="s">
+        <v>522</v>
+      </c>
+      <c r="F20" s="9" t="s">
         <v>523</v>
       </c>
-      <c r="F20" s="9" t="s">
-        <v>452</v>
-      </c>
       <c r="G20" s="9" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9429,10 +9429,10 @@
         <v>2025</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>497</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>498</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>499</v>
       </c>
       <c r="D21" s="9" t="n">
         <v>349</v>
@@ -9441,10 +9441,10 @@
         <v>524</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>452</v>
+        <v>523</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>525</v>
@@ -9455,25 +9455,25 @@
         <v>2025</v>
       </c>
       <c r="B22" s="9" t="s">
+        <v>497</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>498</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>499</v>
       </c>
       <c r="D22" s="9" t="n">
         <v>151</v>
       </c>
       <c r="E22" s="9" t="s">
+        <v>514</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>523</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="H22" s="9" t="s">
         <v>515</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>452</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>510</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>516</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update with legal cases
</commit_message>
<xml_diff>
--- a/CV.xlsx
+++ b/CV.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="737">
   <si>
     <t xml:space="preserve">degree</t>
   </si>
@@ -2168,19 +2168,40 @@
     <t xml:space="preserve">Legal Briefs and Testimony</t>
   </si>
   <si>
+    <t xml:space="preserve">Amicus Curiae Brief</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michigan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">People v. Searcy (04-012890-01-FC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Written and Oral Testimony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Washington District Court</t>
+  </si>
+  <si>
+    <t xml:space="preserve">People v. Lynda Mercy, 21-1-00368-37</t>
+  </si>
+  <si>
     <t xml:space="preserve">Written Testimony</t>
   </si>
   <si>
     <t xml:space="preserve">Colorado District Court</t>
   </si>
   <si>
+    <t xml:space="preserve">People v. Martinez-Sarmiento, 23CR2638</t>
+  </si>
+  <si>
+    <t xml:space="preserve">People v. Fielder, Denver County, 23CR5433.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Federal District Court - Northern District of Florida (Pensacola)</t>
   </si>
   <si>
     <t xml:space="preserve">US v. Quinton Pete, 3:22cr48/TKW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amicus Curiae Brief</t>
   </si>
   <si>
     <t xml:space="preserve">Supreme Court of New Jersey</t>
@@ -2240,7 +2261,7 @@
     <numFmt numFmtId="168" formatCode="yyyy\-mm"/>
     <numFmt numFmtId="169" formatCode="yyyy\-m"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2277,12 +2298,6 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2327,7 +2342,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2384,10 +2399,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3800,10 +3811,10 @@
       <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="15" t="n">
+      <c r="C3" s="14" t="n">
         <v>44774</v>
       </c>
-      <c r="D3" s="15" t="n">
+      <c r="D3" s="14" t="n">
         <v>45047</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -3817,10 +3828,10 @@
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="15" t="n">
+      <c r="C4" s="14" t="n">
         <v>44774</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>632</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -3834,10 +3845,10 @@
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="16" t="n">
+      <c r="C5" s="15" t="n">
         <v>44835</v>
       </c>
-      <c r="D5" s="15" t="n">
+      <c r="D5" s="14" t="n">
         <v>45047</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -3851,7 +3862,7 @@
       <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="15" t="n">
+      <c r="C6" s="14" t="n">
         <v>44409</v>
       </c>
       <c r="D6" s="9" t="s">
@@ -4813,15 +4824,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="59.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="9" width="59.94"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4864,7 +4875,7 @@
         <v>709</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>2025</v>
@@ -4875,7 +4886,9 @@
       <c r="F2" s="1" t="s">
         <v>711</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>712</v>
+      </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -4883,90 +4896,92 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="A3" s="6" t="b">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>709</v>
       </c>
-      <c r="C3" s="11" t="n">
-        <v>2023</v>
-      </c>
-      <c r="D3" s="11" t="n">
-        <v>2023</v>
+      <c r="C3" s="1" t="n">
+        <v>2025</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>2026</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>710</v>
+        <v>713</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>713</v>
-      </c>
+        <v>715</v>
+      </c>
+      <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="b">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>709</v>
       </c>
-      <c r="C4" s="11" t="n">
-        <v>2022</v>
-      </c>
-      <c r="D4" s="11" t="n">
-        <v>2022</v>
+      <c r="C4" s="1" t="n">
+        <v>2025</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>2026</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>716</v>
-      </c>
+        <v>718</v>
+      </c>
+      <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="b">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>709</v>
       </c>
-      <c r="C5" s="11" t="n">
-        <v>2022</v>
-      </c>
-      <c r="D5" s="11" t="n">
-        <v>2022</v>
+      <c r="C5" s="1" t="n">
+        <v>2024</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>2025</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>717</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>718</v>
-      </c>
+        <v>719</v>
+      </c>
+      <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -4975,19 +4990,19 @@
         <v>709</v>
       </c>
       <c r="C6" s="11" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="D6" s="11" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>710</v>
+        <v>716</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -5003,21 +5018,20 @@
         <v>709</v>
       </c>
       <c r="C7" s="11" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="D7" s="11" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>710</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>721</v>
-      </c>
-      <c r="H7" s="1"/>
+        <v>723</v>
+      </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -5029,16 +5043,16 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>722</v>
+        <v>709</v>
       </c>
       <c r="C8" s="11" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="D8" s="11" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>723</v>
+        <v>710</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>724</v>
@@ -5046,7 +5060,6 @@
       <c r="G8" s="1" t="s">
         <v>725</v>
       </c>
-      <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -5058,24 +5071,23 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>722</v>
+        <v>709</v>
       </c>
       <c r="C9" s="11" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="D9" s="11" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>351</v>
+        <v>716</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>726</v>
-      </c>
-      <c r="H9" s="1"/>
+        <v>727</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -5087,39 +5099,52 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>722</v>
+        <v>709</v>
       </c>
       <c r="C10" s="11" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D10" s="11" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>727</v>
+        <v>716</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>728</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>729</v>
-      </c>
+      <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="A11" s="7" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="C11" s="11" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D11" s="11" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>732</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -5127,13 +5152,28 @@
       <c r="L11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="A12" s="7" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="C12" s="11" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D12" s="11" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>733</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -5141,14 +5181,31 @@
       <c r="L12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="A13" s="7" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="C13" s="11" t="n">
+        <v>2020</v>
+      </c>
+      <c r="D13" s="11" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>736</v>
+      </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -5168,7 +5225,7 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -5210,7 +5267,7 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -5224,6 +5281,49 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -6428,13 +6528,13 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="K14" s="0" t="s">
+      <c r="K14" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="L14" s="0" t="n">
+      <c r="L14" s="9" t="n">
         <v>2025</v>
       </c>
-      <c r="M14" s="0" t="n">
+      <c r="M14" s="9" t="n">
         <v>2030</v>
       </c>
     </row>
@@ -8904,7 +9004,7 @@
       <c r="A50" s="5" t="n">
         <v>45873</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="9" t="s">
         <v>202</v>
       </c>
       <c r="C50" s="9" t="s">
@@ -8916,16 +9016,16 @@
       <c r="E50" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="F50" s="0" t="s">
+      <c r="F50" s="9" t="s">
         <v>488</v>
       </c>
-      <c r="G50" s="0" t="s">
+      <c r="G50" s="9" t="s">
         <v>489</v>
       </c>
-      <c r="H50" s="0" t="s">
+      <c r="H50" s="9" t="s">
         <v>490</v>
       </c>
-      <c r="I50" s="0" t="s">
+      <c r="I50" s="9" t="s">
         <v>491</v>
       </c>
       <c r="J50" s="9" t="s">
@@ -8942,7 +9042,7 @@
       <c r="A51" s="5" t="n">
         <v>45878</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="9" t="s">
         <v>202</v>
       </c>
       <c r="C51" s="9" t="s">
@@ -8954,22 +9054,22 @@
       <c r="E51" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="F51" s="0" t="s">
+      <c r="F51" s="9" t="s">
         <v>495</v>
       </c>
-      <c r="H51" s="0" t="s">
+      <c r="H51" s="9" t="s">
         <v>496</v>
       </c>
-      <c r="I51" s="0" t="s">
+      <c r="I51" s="9" t="s">
         <v>497</v>
       </c>
       <c r="J51" s="9" t="s">
         <v>498</v>
       </c>
-      <c r="K51" s="0" t="s">
+      <c r="K51" s="9" t="s">
         <v>499</v>
       </c>
-      <c r="L51" s="0" t="s">
+      <c r="L51" s="9" t="s">
         <v>500</v>
       </c>
     </row>
@@ -9118,7 +9218,7 @@
       <c r="E4" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="1" t="s">
         <v>517</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -9147,7 +9247,7 @@
       <c r="E5" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="1" t="s">
         <v>517</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -9179,7 +9279,7 @@
       <c r="E6" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="1" t="s">
         <v>517</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -9208,7 +9308,7 @@
       <c r="E7" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="1" t="s">
         <v>517</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -9240,7 +9340,7 @@
       <c r="E8" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="1" t="s">
         <v>517</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -9269,7 +9369,7 @@
       <c r="E9" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="1" t="s">
         <v>517</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -9298,7 +9398,7 @@
       <c r="E10" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="1" t="s">
         <v>517</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -9330,7 +9430,7 @@
       <c r="E11" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="1" t="s">
         <v>517</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -9359,7 +9459,7 @@
       <c r="E12" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="1" t="s">
         <v>517</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -9391,7 +9491,7 @@
       <c r="E13" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="1" t="s">
         <v>517</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -9423,7 +9523,7 @@
       <c r="E14" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="1" t="s">
         <v>517</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -9455,7 +9555,7 @@
       <c r="E15" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="1" t="s">
         <v>517</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -9487,16 +9587,16 @@
       <c r="E16" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="1" t="s">
         <v>517</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="I16" s="0" t="n">
+      <c r="I16" s="9" t="n">
         <v>4.45</v>
       </c>
-      <c r="J16" s="0" t="n">
+      <c r="J16" s="9" t="n">
         <v>4.5</v>
       </c>
     </row>
@@ -9516,7 +9616,7 @@
       <c r="E17" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="1" t="s">
         <v>517</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -9525,10 +9625,10 @@
       <c r="H17" s="12" t="s">
         <v>529</v>
       </c>
-      <c r="I17" s="0" t="n">
+      <c r="I17" s="9" t="n">
         <v>4.5</v>
       </c>
-      <c r="J17" s="0" t="n">
+      <c r="J17" s="9" t="n">
         <v>4.625</v>
       </c>
     </row>
@@ -9548,7 +9648,7 @@
       <c r="E18" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="1" t="s">
         <v>517</v>
       </c>
       <c r="G18" s="1" t="s">
@@ -9557,10 +9657,10 @@
       <c r="H18" s="12" t="s">
         <v>532</v>
       </c>
-      <c r="I18" s="0" t="n">
+      <c r="I18" s="9" t="n">
         <v>4.6875</v>
       </c>
-      <c r="J18" s="0" t="n">
+      <c r="J18" s="9" t="n">
         <v>4.75</v>
       </c>
     </row>
@@ -9580,7 +9680,7 @@
       <c r="E19" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="1" t="s">
         <v>517</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -9608,16 +9708,16 @@
       <c r="E20" s="9" t="s">
         <v>536</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="1" t="s">
         <v>517</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>525</v>
       </c>
-      <c r="I20" s="0" t="n">
+      <c r="I20" s="9" t="n">
         <v>4.82</v>
       </c>
-      <c r="J20" s="0" t="n">
+      <c r="J20" s="9" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9637,7 +9737,7 @@
       <c r="E21" s="9" t="s">
         <v>537</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="1" t="s">
         <v>517</v>
       </c>
       <c r="G21" s="9" t="s">
@@ -9646,10 +9746,10 @@
       <c r="H21" s="9" t="s">
         <v>538</v>
       </c>
-      <c r="I21" s="0" t="n">
+      <c r="I21" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="J21" s="0" t="n">
+      <c r="J21" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -9669,7 +9769,7 @@
       <c r="E22" s="9" t="s">
         <v>528</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="1" t="s">
         <v>517</v>
       </c>
       <c r="G22" s="9" t="s">
@@ -9678,62 +9778,62 @@
       <c r="H22" s="9" t="s">
         <v>529</v>
       </c>
-      <c r="I22" s="0" t="n">
+      <c r="I22" s="9" t="n">
         <v>3.903</v>
       </c>
-      <c r="J22" s="0" t="n">
+      <c r="J22" s="9" t="n">
         <v>3.815</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+      <c r="A23" s="9" t="n">
         <v>2025</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="9" t="s">
         <v>515</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>511</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="9" t="n">
         <v>351</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="E23" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="1" t="s">
         <v>517</v>
       </c>
       <c r="G23" s="9" t="s">
         <v>525</v>
       </c>
-      <c r="H23" s="0" t="s">
+      <c r="H23" s="9" t="s">
         <v>540</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+      <c r="A24" s="9" t="n">
         <v>2025</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="9" t="s">
         <v>515</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>511</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="9" t="n">
         <v>850</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="E24" s="9" t="s">
         <v>516</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="1" t="s">
         <v>517</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>523</v>
       </c>
-      <c r="H24" s="0" t="s">
+      <c r="H24" s="9" t="s">
         <v>519</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update students and reviewing
</commit_message>
<xml_diff>
--- a/CV.xlsx
+++ b/CV.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Education" sheetId="1" state="visible" r:id="rId2"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="748">
   <si>
     <t xml:space="preserve">degree</t>
   </si>
@@ -2155,6 +2155,9 @@
   </si>
   <si>
     <t xml:space="preserve">Journal of Statistics and Data Science Education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Journal of Open Source Software</t>
   </si>
   <si>
     <t xml:space="preserve">start_date</t>
@@ -2919,7 +2922,7 @@
   </sheetPr>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -3107,7 +3110,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+      <selection pane="bottomLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3662,7 +3665,7 @@
         <v>2024</v>
       </c>
       <c r="E23" s="9" t="n">
-        <v>0</v>
+        <v>2025</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>623</v>
@@ -3705,7 +3708,7 @@
         <v>2024</v>
       </c>
       <c r="E25" s="9" t="n">
-        <v>0</v>
+        <v>2026</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>626</v>
@@ -3777,7 +3780,7 @@
         <v>2024</v>
       </c>
       <c r="E28" s="9" t="n">
-        <v>0</v>
+        <v>2026</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>631</v>
@@ -4546,10 +4549,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H27" activeCellId="0" sqref="H27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4736,6 +4739,14 @@
       </c>
       <c r="B23" s="9" t="s">
         <v>703</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>2026</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>705</v>
       </c>
     </row>
   </sheetData>
@@ -4767,22 +4778,22 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>144</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4797,10 +4808,10 @@
         <v>2023</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4815,10 +4826,10 @@
         <v>2023</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4833,10 +4844,10 @@
         <v>2022</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4851,7 +4862,7 @@
         <v>2020</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4866,10 +4877,10 @@
         <v>2020</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
     </row>
   </sheetData>
@@ -4907,10 +4918,10 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>144</v>
@@ -4919,13 +4930,13 @@
         <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -4937,7 +4948,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>2025</v>
@@ -4946,13 +4957,13 @@
         <v>2025</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -4966,7 +4977,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>2025</v>
@@ -4975,13 +4986,13 @@
         <v>2026</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -4995,7 +5006,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>2025</v>
@@ -5004,13 +5015,13 @@
         <v>2026</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -5024,7 +5035,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>2024</v>
@@ -5033,13 +5044,13 @@
         <v>2025</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -5053,7 +5064,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C6" s="11" t="n">
         <v>2023</v>
@@ -5062,13 +5073,13 @@
         <v>2023</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -5081,7 +5092,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C7" s="11" t="n">
         <v>2022</v>
@@ -5090,13 +5101,13 @@
         <v>2022</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -5109,7 +5120,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C8" s="11" t="n">
         <v>2022</v>
@@ -5118,13 +5129,13 @@
         <v>2022</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -5137,7 +5148,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C9" s="11" t="n">
         <v>2022</v>
@@ -5146,13 +5157,13 @@
         <v>2022</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -5165,7 +5176,7 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C10" s="11" t="n">
         <v>2021</v>
@@ -5174,13 +5185,13 @@
         <v>2021</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -5194,7 +5205,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="C11" s="11" t="n">
         <v>2021</v>
@@ -5203,13 +5214,13 @@
         <v>2021</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -5223,7 +5234,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="C12" s="11" t="n">
         <v>2021</v>
@@ -5235,10 +5246,10 @@
         <v>352</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -5252,7 +5263,7 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="C13" s="11" t="n">
         <v>2020</v>
@@ -5261,16 +5272,16 @@
         <v>2020</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>

</xml_diff>